<commit_message>
Walidacja pików XML zgodnie ze schematem SD
</commit_message>
<xml_diff>
--- a/Schema/PZG_CelPracy.xlsx
+++ b/Schema/PZG_CelPracy.xlsx
@@ -5,40 +5,30 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\xsd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F43A2C-A898-40F7-8280-D79B07132354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D8EF7F3-13B0-4957-9FF4-F2952246B582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{54AC4555-1947-4870-9044-3C8BE1FC5309}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{CE310B6F-7F75-484D-A866-D8A674006EC3}"/>
   </bookViews>
   <sheets>
-    <sheet name="PZG_CelPracy" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{75147A02-CC02-4979-A3EC-3964B8C51529}" name="PZG_CelPracy" type="4" refreshedVersion="0" background="1">
-    <webPr xml="1" sourceData="1" url="C:\!\PZG_CelPracy.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" xr16:uid="{BFE570A3-C0E7-4497-A27D-94BF04EA0582}" name="PZG_CelPracy" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="R:\xsd\PZG_CelPracy.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Kolumna1</t>
   </si>
@@ -58,16 +48,16 @@
     <t>aktualizacja ewidencji gruntów i budynków (EGiB)</t>
   </si>
   <si>
-    <t>utworzenie bazy danych geodezyjnej sieci uzbrojenia terenu (GESUT)</t>
-  </si>
-  <si>
-    <t>aktualizacja bazy danych geodezyjnej sieci uzbrojenia terenu (GESUT)</t>
-  </si>
-  <si>
-    <t>utworzenie bazy danych obiektów topograficznych (BDOT500)</t>
-  </si>
-  <si>
-    <t>aktualizacja bazy danych obiektów topograficznych (BDOT500)</t>
+    <t>utworzenie bazy danych geodezyjnej ewidencji sieci uzbrojenia terenu (GESUT)</t>
+  </si>
+  <si>
+    <t>aktualizacja bazy danych geodezyjnej ewidencji sieci uzbrojenia terenu (GESUT)</t>
+  </si>
+  <si>
+    <t>utworzenie bazy danych obiektów topograficznych o szczegółowości zapewniającej tworzenie standardowych opracowań kartograficznych w skalach 1:500-1:5000 (BDOT500)</t>
+  </si>
+  <si>
+    <t>aktualizacja bazy danych obiektów topograficznych o szczegółowości zapewniającej tworzenie standardowych opracowań kartograficznych w skalach 1:500-1:5000 (BDOT500)</t>
   </si>
   <si>
     <t>utworzenie bazy danych szczegółowych osnów geodezyjnych (BDSOG)</t>
@@ -97,82 +87,19 @@
     <t>rozgraniczenie nieruchomości</t>
   </si>
   <si>
-    <t>wznowienie znaków granicznych/wyznaczenie punktów/ustalenie przebiegu granic działek</t>
+    <t>wznowienie znaków granicznych/wyznaczenie punktów/ustalenie przebiegu granic działek ewidencyjnych</t>
   </si>
   <si>
     <t>mapa do celów projektowych</t>
   </si>
   <si>
-    <t>geodezyjna inwentaryzacja powykonawcza obiektów budowlanych</t>
-  </si>
-  <si>
-    <t>tyczenie obiektów budowlanych</t>
+    <t>geodezyjna inwentaryzacja obiektów budowlanych</t>
+  </si>
+  <si>
+    <t>wytyczenie obiektów budowlanych</t>
   </si>
   <si>
     <t>inny cel</t>
-  </si>
-  <si>
-    <t>zalozenieEGiB</t>
-  </si>
-  <si>
-    <t>modernizacjaEGiB</t>
-  </si>
-  <si>
-    <t>aktualizacjaEGiB</t>
-  </si>
-  <si>
-    <t>utworzenieGESUT</t>
-  </si>
-  <si>
-    <t>aktualizacjaGESUT</t>
-  </si>
-  <si>
-    <t>utworzenieBDOT500</t>
-  </si>
-  <si>
-    <t>aktualizacjaBDOT500</t>
-  </si>
-  <si>
-    <t>utworzenieBDSOG</t>
-  </si>
-  <si>
-    <t>aktualizacjaBDSOG</t>
-  </si>
-  <si>
-    <t>mapaZProjPodzialu</t>
-  </si>
-  <si>
-    <t>mapaZProjPodzialuRL</t>
-  </si>
-  <si>
-    <t>mapaZProjScalenia</t>
-  </si>
-  <si>
-    <t>projScaleniaGruntow</t>
-  </si>
-  <si>
-    <t>projWymianyGruntow</t>
-  </si>
-  <si>
-    <t>innaMapaDoCelowPr</t>
-  </si>
-  <si>
-    <t>rozgrNieruchomosci</t>
-  </si>
-  <si>
-    <t>wznZnakowGrWyznPGr</t>
-  </si>
-  <si>
-    <t>mapaDoCelowProj</t>
-  </si>
-  <si>
-    <t>geodInwPowykObBud</t>
-  </si>
-  <si>
-    <t>tyczenieObBud</t>
-  </si>
-  <si>
-    <t>innyCel</t>
   </si>
 </sst>
 </file>
@@ -208,10 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -260,16 +186,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5EC4916-CC51-42B3-8B69-04A9C5992F03}" name="Tabela1" displayName="Tabela1" ref="A1:C43" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:C43" xr:uid="{95DC226C-C677-446E-8191-7899F95960FA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE211C5E-ECA4-4C6A-B62F-3C1F080832CD}" name="Tabela1" displayName="Tabela1" ref="A1:C22" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:C22" xr:uid="{AFE20866-48ED-4602-92F6-4FFC1C377E18}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1CF748DE-5094-438C-B1FA-3B05A06F53B6}" uniqueName="key" name="key">
+    <tableColumn id="1" xr3:uid="{303677F0-2A9F-4264-8E8F-E5DDEA246B86}" uniqueName="key" name="key">
       <xmlColumnPr mapId="1" xpath="/PZG_CelPracy/entry/key" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{21023DD7-DCF9-4239-8480-E68FCCB0624F}" uniqueName="value" name="value">
+    <tableColumn id="2" xr3:uid="{123AAE8D-D656-42C1-AD8C-5A1B72144D0C}" uniqueName="value" name="value">
       <xmlColumnPr mapId="1" xpath="/PZG_CelPracy/entry/value" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7673ADFA-3F8E-4EE0-A782-0E9A470AB82D}" uniqueName="3" name="Kolumna1" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{AA163557-3663-48EA-BDD1-BF54A1DE8144}" uniqueName="3" name="Kolumna1" dataDxfId="0">
       <calculatedColumnFormula>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -574,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +568,7 @@
       </c>
       <c r="C5" t="str">
         <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="utworzenie bazy danych geodezyjnej sieci uzbrojenia terenu (GESUT)"/&gt;</v>
+        <v>&lt;enumeration value="utworzenie bazy danych geodezyjnej ewidencji sieci uzbrojenia terenu (GESUT)"/&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,7 +580,7 @@
       </c>
       <c r="C6" t="str">
         <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="aktualizacja bazy danych geodezyjnej sieci uzbrojenia terenu (GESUT)"/&gt;</v>
+        <v>&lt;enumeration value="aktualizacja bazy danych geodezyjnej ewidencji sieci uzbrojenia terenu (GESUT)"/&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -666,7 +592,7 @@
       </c>
       <c r="C7" t="str">
         <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="utworzenie bazy danych obiektów topograficznych (BDOT500)"/&gt;</v>
+        <v>&lt;enumeration value="utworzenie bazy danych obiektów topograficznych o szczegółowości zapewniającej tworzenie standardowych opracowań kartograficznych w skalach 1:500-1:5000 (BDOT500)"/&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,7 +604,7 @@
       </c>
       <c r="C8" t="str">
         <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="aktualizacja bazy danych obiektów topograficznych (BDOT500)"/&gt;</v>
+        <v>&lt;enumeration value="aktualizacja bazy danych obiektów topograficznych o szczegółowości zapewniającej tworzenie standardowych opracowań kartograficznych w skalach 1:500-1:5000 (BDOT500)"/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -798,7 +724,7 @@
       </c>
       <c r="C18" t="str">
         <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="wznowienie znaków granicznych/wyznaczenie punktów/ustalenie przebiegu granic działek"/&gt;</v>
+        <v>&lt;enumeration value="wznowienie znaków granicznych/wyznaczenie punktów/ustalenie przebiegu granic działek ewidencyjnych"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,7 +748,7 @@
       </c>
       <c r="C20" t="str">
         <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="geodezyjna inwentaryzacja powykonawcza obiektów budowlanych"/&gt;</v>
+        <v>&lt;enumeration value="geodezyjna inwentaryzacja obiektów budowlanych"/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -834,7 +760,7 @@
       </c>
       <c r="C21" t="str">
         <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="tyczenie obiektów budowlanych"/&gt;</v>
+        <v>&lt;enumeration value="wytyczenie obiektów budowlanych"/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -847,195 +773,6 @@
       <c r="C22" t="str">
         <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
         <v>&lt;enumeration value="inny cel"/&gt;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="zalozenieEGiB"/&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="modernizacjaEGiB"/&gt;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="aktualizacjaEGiB"/&gt;</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="utworzenieGESUT"/&gt;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="aktualizacjaGESUT"/&gt;</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="utworzenieBDOT500"/&gt;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="aktualizacjaBDOT500"/&gt;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="utworzenieBDSOG"/&gt;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="aktualizacjaBDSOG"/&gt;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="mapaZProjPodzialu"/&gt;</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="mapaZProjPodzialuRL"/&gt;</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="mapaZProjScalenia"/&gt;</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="projScaleniaGruntow"/&gt;</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="projWymianyGruntow"/&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="innaMapaDoCelowPr"/&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="rozgrNieruchomosci"/&gt;</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="wznZnakowGrWyznPGr"/&gt;</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="mapaDoCelowProj"/&gt;</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="geodInwPowykObBud"/&gt;</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="tyczenieObBud"/&gt;</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="2" t="str">
-        <f>"&lt;enumeration value=""" &amp; Tabela1[[#This Row],[value]] &amp; """/&gt;"</f>
-        <v>&lt;enumeration value="innyCel"/&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>